<commit_message>
Condensed examples into one spreadsheet
</commit_message>
<xml_diff>
--- a/PractiCode/PractiCode/CodeExamples.xlsx
+++ b/PractiCode/PractiCode/CodeExamples.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A16401F7-77F5-43F3-ABF2-331370454605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{73FBC543-04C3-402D-8077-D4A756361374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="python" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="javascript" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Hello World</t>
   </si>
@@ -39,11 +41,57 @@
     <t>Adding two numbers</t>
   </si>
   <si>
-    <t>def addition(num1, num2):_x000D_
+    <t>def add(num1, num2):_x000D_
     return(num1 + num2)</t>
   </si>
   <si>
     <t>Return the sum of two numbers</t>
+  </si>
+  <si>
+    <t>Fibonacci</t>
+  </si>
+  <si>
+    <t>def fibonacci(num):_x000D_
+    if num == 1:_x000D_
+        return 1
+    else:
+        return fibonacci(num - 1) + fibonacci(num - 2)</t>
+  </si>
+  <si>
+    <t>Calculate the nth fibonacci number using recursion</t>
+  </si>
+  <si>
+    <t>print("Hello, World!");</t>
+  </si>
+  <si>
+    <t>function add(num1, num2) {
+    return num1 + num2;
+}</t>
+  </si>
+  <si>
+    <t>def fibonacci(num):_x000D_
+    if num == 1 or num == 2:_x000D_
+        return num_x000D_
+    else:_x000D_
+        return fibonacci(num - 1) + fibonacci(num - 2)</t>
+  </si>
+  <si>
+    <t>function fibonacci(num) {_x000D_
+    if (num == 1 || num == 2) {_x000D_
+        return num;_x000D_
+    } else {_x000D_
+        return fibonacci(num-1) + fibonacci(num-2);_x000D_
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>function fibonacci(num) {_x000D_
+    if (num == 1) {_x000D_
+        return 1;_x000D_
+    } else {
+        return fibonacci(num-1) + fibonacci(num-2);
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -398,16 +446,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
     <col min="3" max="3" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -433,6 +481,133 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="75">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254C0ABF-8EE7-4EFA-8BD9-24BCE78F0390}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="3" max="4" width="60.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="105">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73A110C-AEEA-455B-BDF2-1CF40D42637A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="105">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Libraries and Main functions added to interpreters
</commit_message>
<xml_diff>
--- a/PractiCode/PractiCode/CodeExamples.xlsx
+++ b/PractiCode/PractiCode/CodeExamples.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23003"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B261911C-D17D-47A3-A848-8A32C8A6F63B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB7AE1A0-0554-48C8-83BD-E0F30114D10F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,16 +33,24 @@
     <t>Printing a message to standard output</t>
   </si>
   <si>
-    <t>print('Hello, World!')</t>
-  </si>
-  <si>
-    <t>print("Hello, World!");</t>
-  </si>
-  <si>
-    <t>Console.WriteLine("Hello, World!);</t>
-  </si>
-  <si>
-    <t>System.out.print("Hello, World!");</t>
+    <t>def hello_world():
+    print('Hello, World!')</t>
+  </si>
+  <si>
+    <t>function hello_world() {
+     print("Hello, World!");
+}</t>
+  </si>
+  <si>
+    <t>public static void hello_world()
+{_x000D_
+    Console.WriteLine("Hello, World!");
+}</t>
+  </si>
+  <si>
+    <t>public static void hello_world() {
+    System.out.print("Hello, World!");
+}</t>
   </si>
   <si>
     <t>Adding two numbers</t>
@@ -60,13 +68,13 @@
 }</t>
   </si>
   <si>
-    <t>public int add(int num1, int num2)
+    <t>public static int add(int num1, int num2)_x000D_
 {_x000D_
     return num1 + num2;_x000D_
 }</t>
   </si>
   <si>
-    <t>public int add(int num1, int num2) {_x000D_
+    <t>public static int add(int num1, int num2) {_x000D_
     return num1 + num2;_x000D_
 }</t>
   </si>
@@ -93,7 +101,7 @@
 }</t>
   </si>
   <si>
-    <t>public int fibonacci(num)_x000D_
+    <t>public static int fibonacci(num)_x000D_
 {_x000D_
     if (num == 1 || num == 2) _x000D_
     {_x000D_
@@ -102,16 +110,16 @@
     else_x000D_
     {_x000D_
         return fibonacci(num - 1) + fibonacci(num - 2);_x000D_
-    }
-}</t>
-  </si>
-  <si>
-    <t>public int fibonacci(int num) {
-    if (num == 1 || num == 2) {
-        return num;
-    } else {
-        return fibonacci(num-1) + fibonacci(num-2);
-    }
+    }_x000D_
+}</t>
+  </si>
+  <si>
+    <t>public static int fibonacci(int num) {_x000D_
+    if (num == 1 || num == 2) {_x000D_
+        return num;_x000D_
+    } else {_x000D_
+        return fibonacci(num-1) + fibonacci(num-2);_x000D_
+    }_x000D_
 }</t>
   </si>
 </sst>
@@ -469,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254C0ABF-8EE7-4EFA-8BD9-24BCE78F0390}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -482,23 +490,23 @@
     <col min="6" max="6" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a function to the list
</commit_message>
<xml_diff>
--- a/PractiCode/PractiCode/CodeExamples.xlsx
+++ b/PractiCode/PractiCode/CodeExamples.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23005"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB7AE1A0-0554-48C8-83BD-E0F30114D10F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22D87B20-EB3B-4CBE-A7E5-0CB5A9E1A611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Hello World</t>
   </si>
@@ -60,7 +60,7 @@
   </si>
   <si>
     <t>def add(num1, num2):_x000D_
-    return(num1 + num2)</t>
+    return num1 + num2</t>
   </si>
   <si>
     <t>function add(num1, num2) {
@@ -76,6 +76,32 @@
   <si>
     <t>public static int add(int num1, int num2) {_x000D_
     return num1 + num2;_x000D_
+}</t>
+  </si>
+  <si>
+    <t>Multiplying two numbers</t>
+  </si>
+  <si>
+    <t>Return the product of two numbers</t>
+  </si>
+  <si>
+    <t>def multiply(num1, num2):
+    return num1 * num2</t>
+  </si>
+  <si>
+    <t>function multiply(num1, num2) {
+    return num1 * num2;
+}</t>
+  </si>
+  <si>
+    <t>public static int multiply(int num1, int num2)
+{
+    return num1 * num2;
+}</t>
+  </si>
+  <si>
+    <t>public static int multiply(int num1, int num2) {
+    return num1 * num2;
 }</t>
   </si>
   <si>
@@ -101,7 +127,7 @@
 }</t>
   </si>
   <si>
-    <t>public static int fibonacci(num)_x000D_
+    <t>public static int fibonacci(int num)_x000D_
 {_x000D_
     if (num == 1 || num == 2) _x000D_
     {_x000D_
@@ -475,15 +501,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254C0ABF-8EE7-4EFA-8BD9-24BCE78F0390}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.28515625" customWidth="1"/>
     <col min="3" max="4" width="60.5703125" customWidth="1"/>
     <col min="5" max="5" width="47.140625" bestFit="1" customWidth="1"/>
@@ -530,7 +556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="165">
+    <row r="3" spans="1:6" ht="60">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -548,6 +574,26 @@
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="165">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>